<commit_message>
Edited tests and pages
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16680" windowHeight="9315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="824">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1410,13 +1411,1091 @@
   </si>
   <si>
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
+  </si>
+  <si>
+    <t>950b15b</t>
+  </si>
+  <si>
+    <t>2f10a24</t>
+  </si>
+  <si>
+    <t>90a9a2e</t>
+  </si>
+  <si>
+    <t>9c11be2</t>
+  </si>
+  <si>
+    <t>f9246ae</t>
+  </si>
+  <si>
+    <t>2fc8070</t>
+  </si>
+  <si>
+    <t>677ad98</t>
+  </si>
+  <si>
+    <t>340ab0f</t>
+  </si>
+  <si>
+    <t>603fc8b</t>
+  </si>
+  <si>
+    <t>e198fb7</t>
+  </si>
+  <si>
+    <t>a83b0ae</t>
+  </si>
+  <si>
+    <t>6995ed6</t>
+  </si>
+  <si>
+    <t>d42601d</t>
+  </si>
+  <si>
+    <t>d54abd9</t>
+  </si>
+  <si>
+    <t>e398602</t>
+  </si>
+  <si>
+    <t>2e8e6f3</t>
+  </si>
+  <si>
+    <t>3db5633</t>
+  </si>
+  <si>
+    <t>5e4f33f</t>
+  </si>
+  <si>
+    <t>3f1ebf7</t>
+  </si>
+  <si>
+    <t>4454979</t>
+  </si>
+  <si>
+    <t>3f0f7f4</t>
+  </si>
+  <si>
+    <t>9dc717a</t>
+  </si>
+  <si>
+    <t>e512396</t>
+  </si>
+  <si>
+    <t>d863815</t>
+  </si>
+  <si>
+    <t>882bfa8</t>
+  </si>
+  <si>
+    <t>f72a5a2</t>
+  </si>
+  <si>
+    <t>7f31da0</t>
+  </si>
+  <si>
+    <t>d99c169</t>
+  </si>
+  <si>
+    <t>2613fd3</t>
+  </si>
+  <si>
+    <t>c2723ea</t>
+  </si>
+  <si>
+    <t>85b6868</t>
+  </si>
+  <si>
+    <t>32cc9f8</t>
+  </si>
+  <si>
+    <t>cd78dea</t>
+  </si>
+  <si>
+    <t>906c789</t>
+  </si>
+  <si>
+    <t>a3207dd</t>
+  </si>
+  <si>
+    <t>39e8836</t>
+  </si>
+  <si>
+    <t>38f413c</t>
+  </si>
+  <si>
+    <t>c22d070</t>
+  </si>
+  <si>
+    <t>8648b09</t>
+  </si>
+  <si>
+    <t>51bfcf4</t>
+  </si>
+  <si>
+    <t>94b5c30</t>
+  </si>
+  <si>
+    <t>c3136c3</t>
+  </si>
+  <si>
+    <t>9807554</t>
+  </si>
+  <si>
+    <t>ce39f44</t>
+  </si>
+  <si>
+    <t>64781c2</t>
+  </si>
+  <si>
+    <t>845a309</t>
+  </si>
+  <si>
+    <t>b97bfaa</t>
+  </si>
+  <si>
+    <t>f081bbf</t>
+  </si>
+  <si>
+    <t>e592fb7</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>Favourite Category</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>DOGS</t>
+  </si>
+  <si>
+    <t>REPTILES</t>
+  </si>
+  <si>
+    <t>CATS</t>
+  </si>
+  <si>
+    <t>BIRDS</t>
+  </si>
+  <si>
+    <t>f0a61f6</t>
+  </si>
+  <si>
+    <t>208d026</t>
+  </si>
+  <si>
+    <t>bd6998f</t>
+  </si>
+  <si>
+    <t>65d0be1</t>
+  </si>
+  <si>
+    <t>53d4311</t>
+  </si>
+  <si>
+    <t>204c30f</t>
+  </si>
+  <si>
+    <t>eb379f8</t>
+  </si>
+  <si>
+    <t>f36cb1d</t>
+  </si>
+  <si>
+    <t>8604438</t>
+  </si>
+  <si>
+    <t>ef5751b</t>
+  </si>
+  <si>
+    <t>dd2eea5</t>
+  </si>
+  <si>
+    <t>de1e6c2</t>
+  </si>
+  <si>
+    <t>514d527</t>
+  </si>
+  <si>
+    <t>71c0143</t>
+  </si>
+  <si>
+    <t>dfc1102</t>
+  </si>
+  <si>
+    <t>25450ee</t>
+  </si>
+  <si>
+    <t>10a1d8a</t>
+  </si>
+  <si>
+    <t>b0f21af</t>
+  </si>
+  <si>
+    <t>afe20f8</t>
+  </si>
+  <si>
+    <t>b800995</t>
+  </si>
+  <si>
+    <t>bf364d1</t>
+  </si>
+  <si>
+    <t>b1d9143</t>
+  </si>
+  <si>
+    <t>7d47250</t>
+  </si>
+  <si>
+    <t>5bb6a08</t>
+  </si>
+  <si>
+    <t>eba86be</t>
+  </si>
+  <si>
+    <t>5355a95</t>
+  </si>
+  <si>
+    <t>4cd7271</t>
+  </si>
+  <si>
+    <t>d062a74</t>
+  </si>
+  <si>
+    <t>bb787ce</t>
+  </si>
+  <si>
+    <t>f64454a</t>
+  </si>
+  <si>
+    <t>a04335a</t>
+  </si>
+  <si>
+    <t>936c375</t>
+  </si>
+  <si>
+    <t>dbf7532</t>
+  </si>
+  <si>
+    <t>9a889c7</t>
+  </si>
+  <si>
+    <t>bb796ae</t>
+  </si>
+  <si>
+    <t>50b858f</t>
+  </si>
+  <si>
+    <t>4033dd1</t>
+  </si>
+  <si>
+    <t>d97b39d</t>
+  </si>
+  <si>
+    <t>7998841</t>
+  </si>
+  <si>
+    <t>ddf2b7b</t>
+  </si>
+  <si>
+    <t>bb831f0</t>
+  </si>
+  <si>
+    <t>56ec929</t>
+  </si>
+  <si>
+    <t>5c90e0e</t>
+  </si>
+  <si>
+    <t>75d56f9</t>
+  </si>
+  <si>
+    <t>cf17205</t>
+  </si>
+  <si>
+    <t>5da8763</t>
+  </si>
+  <si>
+    <t>90d3146</t>
+  </si>
+  <si>
+    <t>0fde1aa</t>
+  </si>
+  <si>
+    <t>3fdb307</t>
+  </si>
+  <si>
+    <t>ca9c8ec</t>
+  </si>
+  <si>
+    <t>489e6c2</t>
+  </si>
+  <si>
+    <t>d355b37</t>
+  </si>
+  <si>
+    <t>e837309</t>
+  </si>
+  <si>
+    <t>2fdadaa</t>
+  </si>
+  <si>
+    <t>670f13e</t>
+  </si>
+  <si>
+    <t>eaf93cd</t>
+  </si>
+  <si>
+    <t>a606f87</t>
+  </si>
+  <si>
+    <t>60a2b4c</t>
+  </si>
+  <si>
+    <t>fe13cb1</t>
+  </si>
+  <si>
+    <t>f2e20d0</t>
+  </si>
+  <si>
+    <t>484ae64</t>
+  </si>
+  <si>
+    <t>4648186</t>
+  </si>
+  <si>
+    <t>d778b88</t>
+  </si>
+  <si>
+    <t>d29c11b</t>
+  </si>
+  <si>
+    <t>b44a677</t>
+  </si>
+  <si>
+    <t>9238af1</t>
+  </si>
+  <si>
+    <t>5ceb69b</t>
+  </si>
+  <si>
+    <t>8bc6db1</t>
+  </si>
+  <si>
+    <t>326ddf0</t>
+  </si>
+  <si>
+    <t>da4f40c</t>
+  </si>
+  <si>
+    <t>b0ae84a</t>
+  </si>
+  <si>
+    <t>e451e09</t>
+  </si>
+  <si>
+    <t>4a00e41</t>
+  </si>
+  <si>
+    <t>64db283</t>
+  </si>
+  <si>
+    <t>2d8cf71</t>
+  </si>
+  <si>
+    <t>84926a7</t>
+  </si>
+  <si>
+    <t>ea3073e</t>
+  </si>
+  <si>
+    <t>027383b</t>
+  </si>
+  <si>
+    <t>a2aa7b4</t>
+  </si>
+  <si>
+    <t>fcd81ae</t>
+  </si>
+  <si>
+    <t>93fe4e8</t>
+  </si>
+  <si>
+    <t>77dc01c</t>
+  </si>
+  <si>
+    <t>6836cb2</t>
+  </si>
+  <si>
+    <t>b8a1368</t>
+  </si>
+  <si>
+    <t>9d996e3</t>
+  </si>
+  <si>
+    <t>567b4f5</t>
+  </si>
+  <si>
+    <t>b4e62dd</t>
+  </si>
+  <si>
+    <t>bfc3f9e</t>
+  </si>
+  <si>
+    <t>ed89d74</t>
+  </si>
+  <si>
+    <t>b1dd78a</t>
+  </si>
+  <si>
+    <t>c991261</t>
+  </si>
+  <si>
+    <t>81df463</t>
+  </si>
+  <si>
+    <t>1e1df75</t>
+  </si>
+  <si>
+    <t>6e51e24</t>
+  </si>
+  <si>
+    <t>15abc02</t>
+  </si>
+  <si>
+    <t>3b84ce1</t>
+  </si>
+  <si>
+    <t>6bd232e</t>
+  </si>
+  <si>
+    <t>ced231f</t>
+  </si>
+  <si>
+    <t>d589e6c</t>
+  </si>
+  <si>
+    <t>cca444e</t>
+  </si>
+  <si>
+    <t>e74fa17</t>
+  </si>
+  <si>
+    <t>3411950</t>
+  </si>
+  <si>
+    <t>79beb09</t>
+  </si>
+  <si>
+    <t>a488c76</t>
+  </si>
+  <si>
+    <t>a96eb21</t>
+  </si>
+  <si>
+    <t>0e01808</t>
+  </si>
+  <si>
+    <t>8852a3a</t>
+  </si>
+  <si>
+    <t>db3ff6f</t>
+  </si>
+  <si>
+    <t>ebb9698</t>
+  </si>
+  <si>
+    <t>82f9c2e</t>
+  </si>
+  <si>
+    <t>3348d29</t>
+  </si>
+  <si>
+    <t>7d224cf</t>
+  </si>
+  <si>
+    <t>3dc9c7e</t>
+  </si>
+  <si>
+    <t>826c4be</t>
+  </si>
+  <si>
+    <t>5fecba6</t>
+  </si>
+  <si>
+    <t>7f2acf2</t>
+  </si>
+  <si>
+    <t>1baee74</t>
+  </si>
+  <si>
+    <t>9e4dd74</t>
+  </si>
+  <si>
+    <t>5779cd9</t>
+  </si>
+  <si>
+    <t>99c73bb</t>
+  </si>
+  <si>
+    <t>6ec2cad</t>
+  </si>
+  <si>
+    <t>df8b983</t>
+  </si>
+  <si>
+    <t>493f157</t>
+  </si>
+  <si>
+    <t>e58c7e2</t>
+  </si>
+  <si>
+    <t>625716b</t>
+  </si>
+  <si>
+    <t>d986e07</t>
+  </si>
+  <si>
+    <t>64b4225</t>
+  </si>
+  <si>
+    <t>0e80daa</t>
+  </si>
+  <si>
+    <t>2405c01</t>
+  </si>
+  <si>
+    <t>9fe0bae</t>
+  </si>
+  <si>
+    <t>9d71f9b</t>
+  </si>
+  <si>
+    <t>525fcb1</t>
+  </si>
+  <si>
+    <t>a8ff3a5</t>
+  </si>
+  <si>
+    <t>d6cba3b</t>
+  </si>
+  <si>
+    <t>bf4178c</t>
+  </si>
+  <si>
+    <t>7c8de2f</t>
+  </si>
+  <si>
+    <t>fc4d377</t>
+  </si>
+  <si>
+    <t>b6846ef</t>
+  </si>
+  <si>
+    <t>5454005</t>
+  </si>
+  <si>
+    <t>dd73846</t>
+  </si>
+  <si>
+    <t>82b7786</t>
+  </si>
+  <si>
+    <t>641d834</t>
+  </si>
+  <si>
+    <t>10cf751</t>
+  </si>
+  <si>
+    <t>1f25589</t>
+  </si>
+  <si>
+    <t>ede9ae0</t>
+  </si>
+  <si>
+    <t>d5890c7</t>
+  </si>
+  <si>
+    <t>109e1b3</t>
+  </si>
+  <si>
+    <t>46d4a8c</t>
+  </si>
+  <si>
+    <t>a665a02</t>
+  </si>
+  <si>
+    <t>b259c29</t>
+  </si>
+  <si>
+    <t>2020e50</t>
+  </si>
+  <si>
+    <t>7fcacc2</t>
+  </si>
+  <si>
+    <t>1bc8a2a</t>
+  </si>
+  <si>
+    <t>55e0a8b</t>
+  </si>
+  <si>
+    <t>aaa4244</t>
+  </si>
+  <si>
+    <t>7e204ee</t>
+  </si>
+  <si>
+    <t>b11fa97</t>
+  </si>
+  <si>
+    <t>a0c8b0e</t>
+  </si>
+  <si>
+    <t>a09a1c2</t>
+  </si>
+  <si>
+    <t>8e052ff</t>
+  </si>
+  <si>
+    <t>f4216a7</t>
+  </si>
+  <si>
+    <t>7455d65</t>
+  </si>
+  <si>
+    <t>7d155f1</t>
+  </si>
+  <si>
+    <t>3743648</t>
+  </si>
+  <si>
+    <t>3915686</t>
+  </si>
+  <si>
+    <t>3399791</t>
+  </si>
+  <si>
+    <t>f4d5eb6</t>
+  </si>
+  <si>
+    <t>1c07a21</t>
+  </si>
+  <si>
+    <t>59146c0</t>
+  </si>
+  <si>
+    <t>9b4b066</t>
+  </si>
+  <si>
+    <t>b6369d0</t>
+  </si>
+  <si>
+    <t>8715376</t>
+  </si>
+  <si>
+    <t>de5340c</t>
+  </si>
+  <si>
+    <t>45d48d5</t>
+  </si>
+  <si>
+    <t>5af4f3a</t>
+  </si>
+  <si>
+    <t>17a6358</t>
+  </si>
+  <si>
+    <t>1d162e1</t>
+  </si>
+  <si>
+    <t>264ee0e</t>
+  </si>
+  <si>
+    <t>74a3ed7</t>
+  </si>
+  <si>
+    <t>098d52d</t>
+  </si>
+  <si>
+    <t>17596e2</t>
+  </si>
+  <si>
+    <t>f551e68</t>
+  </si>
+  <si>
+    <t>0c7c918</t>
+  </si>
+  <si>
+    <t>aa07b0c</t>
+  </si>
+  <si>
+    <t>dd7897d</t>
+  </si>
+  <si>
+    <t>2a9231e</t>
+  </si>
+  <si>
+    <t>594cc32</t>
+  </si>
+  <si>
+    <t>a8ad078</t>
+  </si>
+  <si>
+    <t>bd2a6bb</t>
+  </si>
+  <si>
+    <t>ae84fb3</t>
+  </si>
+  <si>
+    <t>39e9a71</t>
+  </si>
+  <si>
+    <t>3645f63</t>
+  </si>
+  <si>
+    <t>03085f4</t>
+  </si>
+  <si>
+    <t>b77f81c</t>
+  </si>
+  <si>
+    <t>7006f08</t>
+  </si>
+  <si>
+    <t>df7e5ae</t>
+  </si>
+  <si>
+    <t>58e13ca</t>
+  </si>
+  <si>
+    <t>ad2ebef</t>
+  </si>
+  <si>
+    <t>3f3492c</t>
+  </si>
+  <si>
+    <t>7d93e8c</t>
+  </si>
+  <si>
+    <t>e1891a0</t>
+  </si>
+  <si>
+    <t>81c193a</t>
+  </si>
+  <si>
+    <t>a1044aa</t>
+  </si>
+  <si>
+    <t>45fdcf0</t>
+  </si>
+  <si>
+    <t>cb382bd</t>
+  </si>
+  <si>
+    <t>54d127d</t>
+  </si>
+  <si>
+    <t>d49f92a</t>
+  </si>
+  <si>
+    <t>a18cf55</t>
+  </si>
+  <si>
+    <t>4f81132</t>
+  </si>
+  <si>
+    <t>ef6c0b6</t>
+  </si>
+  <si>
+    <t>4997cd0</t>
+  </si>
+  <si>
+    <t>7e68038</t>
+  </si>
+  <si>
+    <t>2901f12</t>
+  </si>
+  <si>
+    <t>0a24739</t>
+  </si>
+  <si>
+    <t>1a57e2f</t>
+  </si>
+  <si>
+    <t>165fac9</t>
+  </si>
+  <si>
+    <t>7a2f8d7</t>
+  </si>
+  <si>
+    <t>c26fdb8</t>
+  </si>
+  <si>
+    <t>bbe35ac</t>
+  </si>
+  <si>
+    <t>1368d96</t>
+  </si>
+  <si>
+    <t>8cb4aa2</t>
+  </si>
+  <si>
+    <t>02b42ea</t>
+  </si>
+  <si>
+    <t>d096bfe</t>
+  </si>
+  <si>
+    <t>bea4e9c</t>
+  </si>
+  <si>
+    <t>acb3390</t>
+  </si>
+  <si>
+    <t>fdf7445</t>
+  </si>
+  <si>
+    <t>d9b4462</t>
+  </si>
+  <si>
+    <t>74974e6</t>
+  </si>
+  <si>
+    <t>e189a9e</t>
+  </si>
+  <si>
+    <t>d6540c0</t>
+  </si>
+  <si>
+    <t>ef4d46e</t>
+  </si>
+  <si>
+    <t>10b3931</t>
+  </si>
+  <si>
+    <t>9ad4d35</t>
+  </si>
+  <si>
+    <t>32d0399</t>
+  </si>
+  <si>
+    <t>65cb620</t>
+  </si>
+  <si>
+    <t>cc51a99</t>
+  </si>
+  <si>
+    <t>4020013</t>
+  </si>
+  <si>
+    <t>0903832</t>
+  </si>
+  <si>
+    <t>14d58a6</t>
+  </si>
+  <si>
+    <t>cdf6556</t>
+  </si>
+  <si>
+    <t>564d8b1</t>
+  </si>
+  <si>
+    <t>1ec23c5</t>
+  </si>
+  <si>
+    <t>56c2a9d</t>
+  </si>
+  <si>
+    <t>a66c6d7</t>
+  </si>
+  <si>
+    <t>e7ec973</t>
+  </si>
+  <si>
+    <t>6a5185b</t>
+  </si>
+  <si>
+    <t>52c81f5</t>
+  </si>
+  <si>
+    <t>8a9e03b</t>
+  </si>
+  <si>
+    <t>93b80ab</t>
+  </si>
+  <si>
+    <t>f8eed38</t>
+  </si>
+  <si>
+    <t>c0beaa1</t>
+  </si>
+  <si>
+    <t>08a33aa</t>
+  </si>
+  <si>
+    <t>3edebdf</t>
+  </si>
+  <si>
+    <t>b3dd3ee</t>
+  </si>
+  <si>
+    <t>a4d68c6</t>
+  </si>
+  <si>
+    <t>816650c</t>
+  </si>
+  <si>
+    <t>a65ddd0</t>
+  </si>
+  <si>
+    <t>1c00d55</t>
+  </si>
+  <si>
+    <t>4ce4f32</t>
+  </si>
+  <si>
+    <t>788f9eb</t>
+  </si>
+  <si>
+    <t>5bbd0e3</t>
+  </si>
+  <si>
+    <t>5b8cb93</t>
+  </si>
+  <si>
+    <t>be806ce</t>
+  </si>
+  <si>
+    <t>a9205b4</t>
+  </si>
+  <si>
+    <t>7b437ee</t>
+  </si>
+  <si>
+    <t>e6e549f</t>
+  </si>
+  <si>
+    <t>d33f4d5</t>
+  </si>
+  <si>
+    <t>005a3e0</t>
+  </si>
+  <si>
+    <t>af9a59a</t>
+  </si>
+  <si>
+    <t>57380af</t>
+  </si>
+  <si>
+    <t>a63734d</t>
+  </si>
+  <si>
+    <t>8f094ee</t>
+  </si>
+  <si>
+    <t>79ef8cb</t>
+  </si>
+  <si>
+    <t>1b5da09</t>
+  </si>
+  <si>
+    <t>4b407d4</t>
+  </si>
+  <si>
+    <t>eac1469</t>
+  </si>
+  <si>
+    <t>fb8919f</t>
+  </si>
+  <si>
+    <t>3161715</t>
+  </si>
+  <si>
+    <t>ffc2227</t>
+  </si>
+  <si>
+    <t>21775a5</t>
+  </si>
+  <si>
+    <t>69c2c1b</t>
+  </si>
+  <si>
+    <t>94f76f4</t>
+  </si>
+  <si>
+    <t>a7116e8</t>
+  </si>
+  <si>
+    <t>9427387</t>
+  </si>
+  <si>
+    <t>fa8b07e</t>
+  </si>
+  <si>
+    <t>698424f</t>
+  </si>
+  <si>
+    <t>801725f</t>
+  </si>
+  <si>
+    <t>7e30c13</t>
+  </si>
+  <si>
+    <t>90e1b81</t>
+  </si>
+  <si>
+    <t>0c87203</t>
+  </si>
+  <si>
+    <t>e2afa4f</t>
+  </si>
+  <si>
+    <t>8f881d9</t>
+  </si>
+  <si>
+    <t>b2524f8</t>
+  </si>
+  <si>
+    <t>9f9bfb1</t>
+  </si>
+  <si>
+    <t>6e5c38f</t>
+  </si>
+  <si>
+    <t>56a6f53</t>
+  </si>
+  <si>
+    <t>918d593</t>
+  </si>
+  <si>
+    <t>904a3d1</t>
+  </si>
+  <si>
+    <t>fd89bf5</t>
+  </si>
+  <si>
+    <t>401e264</t>
+  </si>
+  <si>
+    <t>dc7146e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1543,7 +2622,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1576,6 +2655,12 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1583,6 +2668,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1661,6 +2751,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1695,6 +2786,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1870,20 +2962,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="108" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>445</v>
       </c>
@@ -1899,7 +2991,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>447</v>
       </c>
@@ -1907,7 +2999,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>449</v>
       </c>
@@ -1915,7 +3007,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>452</v>
       </c>
@@ -1923,7 +3015,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>454</v>
       </c>
@@ -1931,7 +3023,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>455</v>
       </c>
@@ -1939,7 +3031,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>458</v>
       </c>
@@ -1947,7 +3039,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>460</v>
       </c>
@@ -1955,7 +3047,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>462</v>
       </c>
@@ -1963,7 +3055,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>463</v>
       </c>
@@ -1989,23 +3081,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="G36" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="17.28515625" style="3"/>
-    <col min="5" max="5" width="25.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3"/>
-    <col min="7" max="7" width="27.42578125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="17.28515625" style="3"/>
+    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
+    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
+    <col min="8" max="11" style="3" width="17.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="3" width="15.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="14" width="20.5703125" collapsed="true"/>
+    <col min="15" max="16384" style="3" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" thickBot="1">
+    <row r="1" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2042,10 +3138,16 @@
       <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A2" s="4">
-        <v>1</v>
+      <c r="M1" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>774</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2080,10 +3182,16 @@
       <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A3" s="4">
-        <v>2</v>
+      <c r="M2" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>775</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2118,10 +3226,16 @@
       <c r="L3" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A4" s="7">
-        <v>3</v>
+      <c r="M3" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>776</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2156,10 +3270,16 @@
       <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A5" s="4">
-        <v>4</v>
+      <c r="M4" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>777</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2194,10 +3314,16 @@
       <c r="L5" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A6" s="4">
-        <v>5</v>
+      <c r="M5" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>778</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2232,10 +3358,16 @@
       <c r="L6" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A7" s="7">
-        <v>6</v>
+      <c r="M6" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>779</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2270,10 +3402,16 @@
       <c r="L7" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A8" s="4">
-        <v>7</v>
+      <c r="M7" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>780</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2308,10 +3446,16 @@
       <c r="L8" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A9" s="4">
-        <v>8</v>
+      <c r="M8" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>781</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2346,10 +3490,16 @@
       <c r="L9" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A10" s="7">
-        <v>9</v>
+      <c r="M9" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>782</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2384,10 +3534,16 @@
       <c r="L10" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A11" s="4">
-        <v>10</v>
+      <c r="M10" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>783</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2422,10 +3578,16 @@
       <c r="L11" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A12" s="4">
-        <v>11</v>
+      <c r="M11" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>784</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2460,10 +3622,16 @@
       <c r="L12" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A13" s="7">
-        <v>12</v>
+      <c r="M12" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>785</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -2498,10 +3666,16 @@
       <c r="L13" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A14" s="4">
-        <v>13</v>
+      <c r="M13" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>786</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2536,10 +3710,16 @@
       <c r="L14" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A15" s="4">
-        <v>14</v>
+      <c r="M14" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>787</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -2574,10 +3754,16 @@
       <c r="L15" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A16" s="7">
-        <v>15</v>
+      <c r="M15" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>788</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -2612,10 +3798,16 @@
       <c r="L16" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A17" s="4">
-        <v>16</v>
+      <c r="M16" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>789</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -2650,10 +3842,16 @@
       <c r="L17" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A18" s="4">
-        <v>17</v>
+      <c r="M17" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>790</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -2688,10 +3886,16 @@
       <c r="L18" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A19" s="7">
-        <v>18</v>
+      <c r="M18" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>791</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -2726,10 +3930,16 @@
       <c r="L19" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A20" s="4">
-        <v>19</v>
+      <c r="M19" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>792</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -2764,10 +3974,16 @@
       <c r="L20" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A21" s="4">
-        <v>20</v>
+      <c r="M20" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>793</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -2802,10 +4018,16 @@
       <c r="L21" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A22" s="7">
-        <v>21</v>
+      <c r="M21" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>794</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -2840,10 +4062,16 @@
       <c r="L22" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A23" s="4">
-        <v>22</v>
+      <c r="M22" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>795</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -2878,10 +4106,16 @@
       <c r="L23" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A24" s="4">
-        <v>23</v>
+      <c r="M23" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>796</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -2916,10 +4150,16 @@
       <c r="L24" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A25" s="7">
-        <v>24</v>
+      <c r="M24" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>797</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -2954,10 +4194,16 @@
       <c r="L25" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A26" s="4">
-        <v>25</v>
+      <c r="M25" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>798</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -2992,10 +4238,16 @@
       <c r="L26" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A27" s="4">
-        <v>26</v>
+      <c r="M26" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>799</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3030,10 +4282,16 @@
       <c r="L27" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A28" s="7">
-        <v>27</v>
+      <c r="M27" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>800</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3068,10 +4326,16 @@
       <c r="L28" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A29" s="4">
-        <v>28</v>
+      <c r="M28" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>801</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3106,10 +4370,16 @@
       <c r="L29" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A30" s="4">
-        <v>29</v>
+      <c r="M29" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>802</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3144,10 +4414,16 @@
       <c r="L30" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A31" s="7">
-        <v>30</v>
+      <c r="M30" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>803</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3182,10 +4458,16 @@
       <c r="L31" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A32" s="4">
-        <v>31</v>
+      <c r="M31" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>804</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3220,10 +4502,16 @@
       <c r="L32" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A33" s="4">
-        <v>32</v>
+      <c r="M32" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N32" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>805</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3258,10 +4546,16 @@
       <c r="L33" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A34" s="7">
-        <v>33</v>
+      <c r="M33" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N33" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>806</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3296,10 +4590,16 @@
       <c r="L34" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A35" s="4">
-        <v>34</v>
+      <c r="M34" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>807</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3334,10 +4634,16 @@
       <c r="L35" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A36" s="4">
-        <v>35</v>
+      <c r="M35" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>808</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3372,10 +4678,16 @@
       <c r="L36" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A37" s="7">
-        <v>36</v>
+      <c r="M36" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>809</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -3410,10 +4722,16 @@
       <c r="L37" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A38" s="4">
-        <v>37</v>
+      <c r="M37" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>810</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -3448,10 +4766,16 @@
       <c r="L38" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A39" s="4">
-        <v>38</v>
+      <c r="M38" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>811</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -3486,10 +4810,16 @@
       <c r="L39" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A40" s="7">
-        <v>39</v>
+      <c r="M39" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>812</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -3524,10 +4854,16 @@
       <c r="L40" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A41" s="4">
-        <v>40</v>
+      <c r="M40" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>813</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -3562,10 +4898,16 @@
       <c r="L41" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A42" s="4">
-        <v>41</v>
+      <c r="M41" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>814</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -3600,10 +4942,16 @@
       <c r="L42" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A43" s="7">
-        <v>42</v>
+      <c r="M42" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>815</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -3638,10 +4986,16 @@
       <c r="L43" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A44" s="4">
-        <v>43</v>
+      <c r="M43" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>816</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -3676,10 +5030,16 @@
       <c r="L44" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A45" s="4">
-        <v>44</v>
+      <c r="M44" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N44" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>817</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -3714,10 +5074,16 @@
       <c r="L45" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A46" s="7">
-        <v>45</v>
+      <c r="M45" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N45" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>818</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -3752,10 +5118,16 @@
       <c r="L46" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="58.5" thickBot="1">
-      <c r="A47" s="4">
-        <v>46</v>
+      <c r="M46" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N46" s="8" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>819</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -3790,10 +5162,16 @@
       <c r="L47" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A48" s="4">
-        <v>47</v>
+      <c r="M47" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>820</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -3828,10 +5206,16 @@
       <c r="L48" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A49" s="7">
-        <v>48</v>
+      <c r="M48" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>821</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -3866,10 +5250,16 @@
       <c r="L49" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A50" s="4">
-        <v>49</v>
+      <c r="M49" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>822</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -3904,10 +5294,16 @@
       <c r="L50" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="44.25" thickBot="1">
-      <c r="A51" s="4">
-        <v>50</v>
+      <c r="M50" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>823</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -3941,6 +5337,12 @@
       </c>
       <c r="L51" s="5" t="s">
         <v>23</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="N51" s="8" t="s">
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited pages,tests and some files
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16680" windowHeight="9315" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16695" windowHeight="9165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cart_items" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="524">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1413,153 +1413,6 @@
     <t>https://petstore.octoperf.com/actions/Catalog.action?viewItem=&amp;itemId=EST-13</t>
   </si>
   <si>
-    <t>950b15b</t>
-  </si>
-  <si>
-    <t>2f10a24</t>
-  </si>
-  <si>
-    <t>90a9a2e</t>
-  </si>
-  <si>
-    <t>9c11be2</t>
-  </si>
-  <si>
-    <t>f9246ae</t>
-  </si>
-  <si>
-    <t>2fc8070</t>
-  </si>
-  <si>
-    <t>677ad98</t>
-  </si>
-  <si>
-    <t>340ab0f</t>
-  </si>
-  <si>
-    <t>603fc8b</t>
-  </si>
-  <si>
-    <t>e198fb7</t>
-  </si>
-  <si>
-    <t>a83b0ae</t>
-  </si>
-  <si>
-    <t>6995ed6</t>
-  </si>
-  <si>
-    <t>d42601d</t>
-  </si>
-  <si>
-    <t>d54abd9</t>
-  </si>
-  <si>
-    <t>e398602</t>
-  </si>
-  <si>
-    <t>2e8e6f3</t>
-  </si>
-  <si>
-    <t>3db5633</t>
-  </si>
-  <si>
-    <t>5e4f33f</t>
-  </si>
-  <si>
-    <t>3f1ebf7</t>
-  </si>
-  <si>
-    <t>4454979</t>
-  </si>
-  <si>
-    <t>3f0f7f4</t>
-  </si>
-  <si>
-    <t>9dc717a</t>
-  </si>
-  <si>
-    <t>e512396</t>
-  </si>
-  <si>
-    <t>d863815</t>
-  </si>
-  <si>
-    <t>882bfa8</t>
-  </si>
-  <si>
-    <t>f72a5a2</t>
-  </si>
-  <si>
-    <t>7f31da0</t>
-  </si>
-  <si>
-    <t>d99c169</t>
-  </si>
-  <si>
-    <t>2613fd3</t>
-  </si>
-  <si>
-    <t>c2723ea</t>
-  </si>
-  <si>
-    <t>85b6868</t>
-  </si>
-  <si>
-    <t>32cc9f8</t>
-  </si>
-  <si>
-    <t>cd78dea</t>
-  </si>
-  <si>
-    <t>906c789</t>
-  </si>
-  <si>
-    <t>a3207dd</t>
-  </si>
-  <si>
-    <t>39e8836</t>
-  </si>
-  <si>
-    <t>38f413c</t>
-  </si>
-  <si>
-    <t>c22d070</t>
-  </si>
-  <si>
-    <t>8648b09</t>
-  </si>
-  <si>
-    <t>51bfcf4</t>
-  </si>
-  <si>
-    <t>94b5c30</t>
-  </si>
-  <si>
-    <t>c3136c3</t>
-  </si>
-  <si>
-    <t>9807554</t>
-  </si>
-  <si>
-    <t>ce39f44</t>
-  </si>
-  <si>
-    <t>64781c2</t>
-  </si>
-  <si>
-    <t>845a309</t>
-  </si>
-  <si>
-    <t>b97bfaa</t>
-  </si>
-  <si>
-    <t>f081bbf</t>
-  </si>
-  <si>
-    <t>e592fb7</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -1585,759 +1438,6 @@
   </si>
   <si>
     <t>BIRDS</t>
-  </si>
-  <si>
-    <t>f0a61f6</t>
-  </si>
-  <si>
-    <t>208d026</t>
-  </si>
-  <si>
-    <t>bd6998f</t>
-  </si>
-  <si>
-    <t>65d0be1</t>
-  </si>
-  <si>
-    <t>53d4311</t>
-  </si>
-  <si>
-    <t>204c30f</t>
-  </si>
-  <si>
-    <t>eb379f8</t>
-  </si>
-  <si>
-    <t>f36cb1d</t>
-  </si>
-  <si>
-    <t>8604438</t>
-  </si>
-  <si>
-    <t>ef5751b</t>
-  </si>
-  <si>
-    <t>dd2eea5</t>
-  </si>
-  <si>
-    <t>de1e6c2</t>
-  </si>
-  <si>
-    <t>514d527</t>
-  </si>
-  <si>
-    <t>71c0143</t>
-  </si>
-  <si>
-    <t>dfc1102</t>
-  </si>
-  <si>
-    <t>25450ee</t>
-  </si>
-  <si>
-    <t>10a1d8a</t>
-  </si>
-  <si>
-    <t>b0f21af</t>
-  </si>
-  <si>
-    <t>afe20f8</t>
-  </si>
-  <si>
-    <t>b800995</t>
-  </si>
-  <si>
-    <t>bf364d1</t>
-  </si>
-  <si>
-    <t>b1d9143</t>
-  </si>
-  <si>
-    <t>7d47250</t>
-  </si>
-  <si>
-    <t>5bb6a08</t>
-  </si>
-  <si>
-    <t>eba86be</t>
-  </si>
-  <si>
-    <t>5355a95</t>
-  </si>
-  <si>
-    <t>4cd7271</t>
-  </si>
-  <si>
-    <t>d062a74</t>
-  </si>
-  <si>
-    <t>bb787ce</t>
-  </si>
-  <si>
-    <t>f64454a</t>
-  </si>
-  <si>
-    <t>a04335a</t>
-  </si>
-  <si>
-    <t>936c375</t>
-  </si>
-  <si>
-    <t>dbf7532</t>
-  </si>
-  <si>
-    <t>9a889c7</t>
-  </si>
-  <si>
-    <t>bb796ae</t>
-  </si>
-  <si>
-    <t>50b858f</t>
-  </si>
-  <si>
-    <t>4033dd1</t>
-  </si>
-  <si>
-    <t>d97b39d</t>
-  </si>
-  <si>
-    <t>7998841</t>
-  </si>
-  <si>
-    <t>ddf2b7b</t>
-  </si>
-  <si>
-    <t>bb831f0</t>
-  </si>
-  <si>
-    <t>56ec929</t>
-  </si>
-  <si>
-    <t>5c90e0e</t>
-  </si>
-  <si>
-    <t>75d56f9</t>
-  </si>
-  <si>
-    <t>cf17205</t>
-  </si>
-  <si>
-    <t>5da8763</t>
-  </si>
-  <si>
-    <t>90d3146</t>
-  </si>
-  <si>
-    <t>0fde1aa</t>
-  </si>
-  <si>
-    <t>3fdb307</t>
-  </si>
-  <si>
-    <t>ca9c8ec</t>
-  </si>
-  <si>
-    <t>489e6c2</t>
-  </si>
-  <si>
-    <t>d355b37</t>
-  </si>
-  <si>
-    <t>e837309</t>
-  </si>
-  <si>
-    <t>2fdadaa</t>
-  </si>
-  <si>
-    <t>670f13e</t>
-  </si>
-  <si>
-    <t>eaf93cd</t>
-  </si>
-  <si>
-    <t>a606f87</t>
-  </si>
-  <si>
-    <t>60a2b4c</t>
-  </si>
-  <si>
-    <t>fe13cb1</t>
-  </si>
-  <si>
-    <t>f2e20d0</t>
-  </si>
-  <si>
-    <t>484ae64</t>
-  </si>
-  <si>
-    <t>4648186</t>
-  </si>
-  <si>
-    <t>d778b88</t>
-  </si>
-  <si>
-    <t>d29c11b</t>
-  </si>
-  <si>
-    <t>b44a677</t>
-  </si>
-  <si>
-    <t>9238af1</t>
-  </si>
-  <si>
-    <t>5ceb69b</t>
-  </si>
-  <si>
-    <t>8bc6db1</t>
-  </si>
-  <si>
-    <t>326ddf0</t>
-  </si>
-  <si>
-    <t>da4f40c</t>
-  </si>
-  <si>
-    <t>b0ae84a</t>
-  </si>
-  <si>
-    <t>e451e09</t>
-  </si>
-  <si>
-    <t>4a00e41</t>
-  </si>
-  <si>
-    <t>64db283</t>
-  </si>
-  <si>
-    <t>2d8cf71</t>
-  </si>
-  <si>
-    <t>84926a7</t>
-  </si>
-  <si>
-    <t>ea3073e</t>
-  </si>
-  <si>
-    <t>027383b</t>
-  </si>
-  <si>
-    <t>a2aa7b4</t>
-  </si>
-  <si>
-    <t>fcd81ae</t>
-  </si>
-  <si>
-    <t>93fe4e8</t>
-  </si>
-  <si>
-    <t>77dc01c</t>
-  </si>
-  <si>
-    <t>6836cb2</t>
-  </si>
-  <si>
-    <t>b8a1368</t>
-  </si>
-  <si>
-    <t>9d996e3</t>
-  </si>
-  <si>
-    <t>567b4f5</t>
-  </si>
-  <si>
-    <t>b4e62dd</t>
-  </si>
-  <si>
-    <t>bfc3f9e</t>
-  </si>
-  <si>
-    <t>ed89d74</t>
-  </si>
-  <si>
-    <t>b1dd78a</t>
-  </si>
-  <si>
-    <t>c991261</t>
-  </si>
-  <si>
-    <t>81df463</t>
-  </si>
-  <si>
-    <t>1e1df75</t>
-  </si>
-  <si>
-    <t>6e51e24</t>
-  </si>
-  <si>
-    <t>15abc02</t>
-  </si>
-  <si>
-    <t>3b84ce1</t>
-  </si>
-  <si>
-    <t>6bd232e</t>
-  </si>
-  <si>
-    <t>ced231f</t>
-  </si>
-  <si>
-    <t>d589e6c</t>
-  </si>
-  <si>
-    <t>cca444e</t>
-  </si>
-  <si>
-    <t>e74fa17</t>
-  </si>
-  <si>
-    <t>3411950</t>
-  </si>
-  <si>
-    <t>79beb09</t>
-  </si>
-  <si>
-    <t>a488c76</t>
-  </si>
-  <si>
-    <t>a96eb21</t>
-  </si>
-  <si>
-    <t>0e01808</t>
-  </si>
-  <si>
-    <t>8852a3a</t>
-  </si>
-  <si>
-    <t>db3ff6f</t>
-  </si>
-  <si>
-    <t>ebb9698</t>
-  </si>
-  <si>
-    <t>82f9c2e</t>
-  </si>
-  <si>
-    <t>3348d29</t>
-  </si>
-  <si>
-    <t>7d224cf</t>
-  </si>
-  <si>
-    <t>3dc9c7e</t>
-  </si>
-  <si>
-    <t>826c4be</t>
-  </si>
-  <si>
-    <t>5fecba6</t>
-  </si>
-  <si>
-    <t>7f2acf2</t>
-  </si>
-  <si>
-    <t>1baee74</t>
-  </si>
-  <si>
-    <t>9e4dd74</t>
-  </si>
-  <si>
-    <t>5779cd9</t>
-  </si>
-  <si>
-    <t>99c73bb</t>
-  </si>
-  <si>
-    <t>6ec2cad</t>
-  </si>
-  <si>
-    <t>df8b983</t>
-  </si>
-  <si>
-    <t>493f157</t>
-  </si>
-  <si>
-    <t>e58c7e2</t>
-  </si>
-  <si>
-    <t>625716b</t>
-  </si>
-  <si>
-    <t>d986e07</t>
-  </si>
-  <si>
-    <t>64b4225</t>
-  </si>
-  <si>
-    <t>0e80daa</t>
-  </si>
-  <si>
-    <t>2405c01</t>
-  </si>
-  <si>
-    <t>9fe0bae</t>
-  </si>
-  <si>
-    <t>9d71f9b</t>
-  </si>
-  <si>
-    <t>525fcb1</t>
-  </si>
-  <si>
-    <t>a8ff3a5</t>
-  </si>
-  <si>
-    <t>d6cba3b</t>
-  </si>
-  <si>
-    <t>bf4178c</t>
-  </si>
-  <si>
-    <t>7c8de2f</t>
-  </si>
-  <si>
-    <t>fc4d377</t>
-  </si>
-  <si>
-    <t>b6846ef</t>
-  </si>
-  <si>
-    <t>5454005</t>
-  </si>
-  <si>
-    <t>dd73846</t>
-  </si>
-  <si>
-    <t>82b7786</t>
-  </si>
-  <si>
-    <t>641d834</t>
-  </si>
-  <si>
-    <t>10cf751</t>
-  </si>
-  <si>
-    <t>1f25589</t>
-  </si>
-  <si>
-    <t>ede9ae0</t>
-  </si>
-  <si>
-    <t>d5890c7</t>
-  </si>
-  <si>
-    <t>109e1b3</t>
-  </si>
-  <si>
-    <t>46d4a8c</t>
-  </si>
-  <si>
-    <t>a665a02</t>
-  </si>
-  <si>
-    <t>b259c29</t>
-  </si>
-  <si>
-    <t>2020e50</t>
-  </si>
-  <si>
-    <t>7fcacc2</t>
-  </si>
-  <si>
-    <t>1bc8a2a</t>
-  </si>
-  <si>
-    <t>55e0a8b</t>
-  </si>
-  <si>
-    <t>aaa4244</t>
-  </si>
-  <si>
-    <t>7e204ee</t>
-  </si>
-  <si>
-    <t>b11fa97</t>
-  </si>
-  <si>
-    <t>a0c8b0e</t>
-  </si>
-  <si>
-    <t>a09a1c2</t>
-  </si>
-  <si>
-    <t>8e052ff</t>
-  </si>
-  <si>
-    <t>f4216a7</t>
-  </si>
-  <si>
-    <t>7455d65</t>
-  </si>
-  <si>
-    <t>7d155f1</t>
-  </si>
-  <si>
-    <t>3743648</t>
-  </si>
-  <si>
-    <t>3915686</t>
-  </si>
-  <si>
-    <t>3399791</t>
-  </si>
-  <si>
-    <t>f4d5eb6</t>
-  </si>
-  <si>
-    <t>1c07a21</t>
-  </si>
-  <si>
-    <t>59146c0</t>
-  </si>
-  <si>
-    <t>9b4b066</t>
-  </si>
-  <si>
-    <t>b6369d0</t>
-  </si>
-  <si>
-    <t>8715376</t>
-  </si>
-  <si>
-    <t>de5340c</t>
-  </si>
-  <si>
-    <t>45d48d5</t>
-  </si>
-  <si>
-    <t>5af4f3a</t>
-  </si>
-  <si>
-    <t>17a6358</t>
-  </si>
-  <si>
-    <t>1d162e1</t>
-  </si>
-  <si>
-    <t>264ee0e</t>
-  </si>
-  <si>
-    <t>74a3ed7</t>
-  </si>
-  <si>
-    <t>098d52d</t>
-  </si>
-  <si>
-    <t>17596e2</t>
-  </si>
-  <si>
-    <t>f551e68</t>
-  </si>
-  <si>
-    <t>0c7c918</t>
-  </si>
-  <si>
-    <t>aa07b0c</t>
-  </si>
-  <si>
-    <t>dd7897d</t>
-  </si>
-  <si>
-    <t>2a9231e</t>
-  </si>
-  <si>
-    <t>594cc32</t>
-  </si>
-  <si>
-    <t>a8ad078</t>
-  </si>
-  <si>
-    <t>bd2a6bb</t>
-  </si>
-  <si>
-    <t>ae84fb3</t>
-  </si>
-  <si>
-    <t>39e9a71</t>
-  </si>
-  <si>
-    <t>3645f63</t>
-  </si>
-  <si>
-    <t>03085f4</t>
-  </si>
-  <si>
-    <t>b77f81c</t>
-  </si>
-  <si>
-    <t>7006f08</t>
-  </si>
-  <si>
-    <t>df7e5ae</t>
-  </si>
-  <si>
-    <t>58e13ca</t>
-  </si>
-  <si>
-    <t>ad2ebef</t>
-  </si>
-  <si>
-    <t>3f3492c</t>
-  </si>
-  <si>
-    <t>7d93e8c</t>
-  </si>
-  <si>
-    <t>e1891a0</t>
-  </si>
-  <si>
-    <t>81c193a</t>
-  </si>
-  <si>
-    <t>a1044aa</t>
-  </si>
-  <si>
-    <t>45fdcf0</t>
-  </si>
-  <si>
-    <t>cb382bd</t>
-  </si>
-  <si>
-    <t>54d127d</t>
-  </si>
-  <si>
-    <t>d49f92a</t>
-  </si>
-  <si>
-    <t>a18cf55</t>
-  </si>
-  <si>
-    <t>4f81132</t>
-  </si>
-  <si>
-    <t>ef6c0b6</t>
-  </si>
-  <si>
-    <t>4997cd0</t>
-  </si>
-  <si>
-    <t>7e68038</t>
-  </si>
-  <si>
-    <t>2901f12</t>
-  </si>
-  <si>
-    <t>0a24739</t>
-  </si>
-  <si>
-    <t>1a57e2f</t>
-  </si>
-  <si>
-    <t>165fac9</t>
-  </si>
-  <si>
-    <t>7a2f8d7</t>
-  </si>
-  <si>
-    <t>c26fdb8</t>
-  </si>
-  <si>
-    <t>bbe35ac</t>
-  </si>
-  <si>
-    <t>1368d96</t>
-  </si>
-  <si>
-    <t>8cb4aa2</t>
-  </si>
-  <si>
-    <t>02b42ea</t>
-  </si>
-  <si>
-    <t>d096bfe</t>
-  </si>
-  <si>
-    <t>bea4e9c</t>
-  </si>
-  <si>
-    <t>acb3390</t>
-  </si>
-  <si>
-    <t>fdf7445</t>
-  </si>
-  <si>
-    <t>d9b4462</t>
-  </si>
-  <si>
-    <t>74974e6</t>
-  </si>
-  <si>
-    <t>e189a9e</t>
-  </si>
-  <si>
-    <t>d6540c0</t>
-  </si>
-  <si>
-    <t>ef4d46e</t>
-  </si>
-  <si>
-    <t>10b3931</t>
-  </si>
-  <si>
-    <t>9ad4d35</t>
-  </si>
-  <si>
-    <t>32d0399</t>
-  </si>
-  <si>
-    <t>65cb620</t>
-  </si>
-  <si>
-    <t>cc51a99</t>
-  </si>
-  <si>
-    <t>4020013</t>
-  </si>
-  <si>
-    <t>0903832</t>
-  </si>
-  <si>
-    <t>14d58a6</t>
-  </si>
-  <si>
-    <t>cdf6556</t>
-  </si>
-  <si>
-    <t>564d8b1</t>
-  </si>
-  <si>
-    <t>1ec23c5</t>
-  </si>
-  <si>
-    <t>56c2a9d</t>
-  </si>
-  <si>
-    <t>a66c6d7</t>
-  </si>
-  <si>
-    <t>e7ec973</t>
-  </si>
-  <si>
-    <t>6a5185b</t>
-  </si>
-  <si>
-    <t>52c81f5</t>
-  </si>
-  <si>
-    <t>8a9e03b</t>
-  </si>
-  <si>
-    <t>93b80ab</t>
-  </si>
-  <si>
-    <t>f8eed38</t>
-  </si>
-  <si>
-    <t>c0beaa1</t>
   </si>
   <si>
     <t>08a33aa</t>
@@ -2494,7 +1594,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2971,8 +2070,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="108.0" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="108" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3082,23 +2181,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G36" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="H43" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="3" width="17.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="3" width="25.85546875" collapsed="true"/>
-    <col min="6" max="6" style="3" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="3" width="27.42578125" collapsed="true"/>
-    <col min="8" max="11" style="3" width="17.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="3" width="15.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="14" width="20.5703125" collapsed="true"/>
-    <col min="15" max="16384" style="3" width="17.28515625" collapsed="true"/>
+    <col min="1" max="4" width="17.28515625" style="3" collapsed="1"/>
+    <col min="5" max="5" width="25.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" style="3" collapsed="1"/>
+    <col min="7" max="7" width="27.42578125" style="3" customWidth="1" collapsed="1"/>
+    <col min="8" max="11" width="17.28515625" style="3" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" style="14" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.5703125" style="14" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="17.28515625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3139,15 +2238,15 @@
         <v>13</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>514</v>
+        <v>465</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>517</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>774</v>
+        <v>474</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -3183,15 +2282,15 @@
         <v>23</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>775</v>
+        <v>475</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -3227,15 +2326,15 @@
         <v>23</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>776</v>
+        <v>476</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -3271,15 +2370,15 @@
         <v>23</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>777</v>
+        <v>477</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -3315,15 +2414,15 @@
         <v>23</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>778</v>
+        <v>478</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -3359,15 +2458,15 @@
         <v>23</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>779</v>
+        <v>479</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -3403,15 +2502,15 @@
         <v>23</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>780</v>
+        <v>480</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -3447,15 +2546,15 @@
         <v>23</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>781</v>
+        <v>481</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -3491,15 +2590,15 @@
         <v>23</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>782</v>
+        <v>482</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -3535,15 +2634,15 @@
         <v>23</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>783</v>
+        <v>483</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -3579,15 +2678,15 @@
         <v>23</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>784</v>
+        <v>484</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -3623,15 +2722,15 @@
         <v>23</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>785</v>
+        <v>485</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3667,15 +2766,15 @@
         <v>23</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>786</v>
+        <v>486</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3711,15 +2810,15 @@
         <v>23</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>787</v>
+        <v>487</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3755,15 +2854,15 @@
         <v>23</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>788</v>
+        <v>488</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3799,15 +2898,15 @@
         <v>23</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>789</v>
+        <v>489</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3843,15 +2942,15 @@
         <v>23</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>790</v>
+        <v>490</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3887,15 +2986,15 @@
         <v>23</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>791</v>
+        <v>491</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3931,15 +3030,15 @@
         <v>23</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>792</v>
+        <v>492</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3975,15 +3074,15 @@
         <v>23</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>793</v>
+        <v>493</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -4019,15 +3118,15 @@
         <v>23</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>794</v>
+        <v>494</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -4063,15 +3162,15 @@
         <v>23</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>795</v>
+        <v>495</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -4107,15 +3206,15 @@
         <v>23</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N23" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>796</v>
+        <v>496</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -4151,15 +3250,15 @@
         <v>23</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>797</v>
+        <v>497</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -4195,15 +3294,15 @@
         <v>23</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>798</v>
+        <v>498</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -4239,15 +3338,15 @@
         <v>23</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>799</v>
+        <v>499</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -4283,15 +3382,15 @@
         <v>23</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -4327,15 +3426,15 @@
         <v>23</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>801</v>
+        <v>501</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -4371,15 +3470,15 @@
         <v>23</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>802</v>
+        <v>502</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -4415,15 +3514,15 @@
         <v>23</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>803</v>
+        <v>503</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -4459,15 +3558,15 @@
         <v>23</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>804</v>
+        <v>504</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -4503,15 +3602,15 @@
         <v>23</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>805</v>
+        <v>505</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -4547,15 +3646,15 @@
         <v>23</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>806</v>
+        <v>506</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -4591,15 +3690,15 @@
         <v>23</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>807</v>
+        <v>507</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -4635,15 +3734,15 @@
         <v>23</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N35" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>808</v>
+        <v>508</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -4679,15 +3778,15 @@
         <v>23</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N36" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>809</v>
+        <v>509</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4723,15 +3822,15 @@
         <v>23</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N37" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>810</v>
+        <v>510</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4767,15 +3866,15 @@
         <v>23</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>811</v>
+        <v>511</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4811,15 +3910,15 @@
         <v>23</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>812</v>
+        <v>512</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4855,15 +3954,15 @@
         <v>23</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>813</v>
+        <v>513</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4899,15 +3998,15 @@
         <v>23</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>814</v>
+        <v>514</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4943,15 +4042,15 @@
         <v>23</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>815</v>
+        <v>515</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4987,15 +4086,15 @@
         <v>23</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>816</v>
+        <v>516</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -5031,15 +4130,15 @@
         <v>23</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>817</v>
+        <v>517</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -5075,15 +4174,15 @@
         <v>23</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N45" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>818</v>
+        <v>518</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -5119,15 +4218,15 @@
         <v>23</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>515</v>
+        <v>467</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>819</v>
+        <v>519</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -5163,15 +4262,15 @@
         <v>23</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>518</v>
+        <v>469</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>820</v>
+        <v>520</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -5207,15 +4306,15 @@
         <v>23</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>519</v>
+        <v>470</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>821</v>
+        <v>521</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -5251,15 +4350,15 @@
         <v>23</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>520</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>822</v>
+        <v>522</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -5295,15 +4394,15 @@
         <v>23</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>516</v>
+        <v>467</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>521</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>823</v>
+        <v>523</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -5339,10 +4438,10 @@
         <v>23</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>515</v>
+        <v>466</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>522</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>